<commit_message>
Remove .xlsx files after adding to .gitignore
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -441,6 +441,11 @@
           <t>company</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -450,7 +455,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -465,7 +470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +484,59 @@
           <t>location</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>company</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>BC</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>NHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>test123</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>mhfkymh</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>feqF</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NHS</t>
         </is>
       </c>
     </row>
@@ -498,7 +551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,14 +565,82 @@
           <t>asset_type</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>banana</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>cableway</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>hiuewkcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>pppoknl</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>okjhgnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>u54jktyu</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>VDS</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>feqF</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>